<commit_message>
Post-processing with read smps data
</commit_message>
<xml_diff>
--- a/inputs/odias_params.xlsx
+++ b/inputs/odias_params.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\hmdni\OneDrive\Documents\GitHub\odias\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B07B6A3-0CEA-4FAF-8A6D-E46D0BFC7ADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B417DFA0-EC03-4785-AD1A-0D155F95B26A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="3465" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="26&amp;30JUL24" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
   <si>
     <t>fname</t>
   </si>
@@ -156,6 +156,9 @@
   </si>
   <si>
     <t>#A1CCD1</t>
+  </si>
+  <si>
+    <t>dma_params</t>
   </si>
 </sst>
 </file>
@@ -488,7 +491,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E7"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,7 +534,7 @@
     </row>
     <row r="2" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>36</v>

</xml_diff>